<commit_message>
incorporado o modelo de regressão linear com a reta tracejada do estouro de 383 leitos
</commit_message>
<xml_diff>
--- a/Corona/uti_agregado_diario_imputada_adulto.xlsx
+++ b/Corona/uti_agregado_diario_imputada_adulto.xlsx
@@ -6688,43 +6688,87 @@
         <v>44051</v>
       </c>
       <c r="B144" t="n">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="C144" t="n">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D144" t="n">
-        <v>704</v>
+        <v>708</v>
       </c>
       <c r="E144" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F144" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G144" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H144" t="n">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="I144" t="n">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="J144" t="n">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="K144" t="n">
         <v>17</v>
       </c>
       <c r="L144" t="n">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="M144" t="n">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="N144" t="n">
-        <v>370</v>
+        <v>368</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="n">
+        <v>44052</v>
+      </c>
+      <c r="B145" t="n">
+        <v>823</v>
+      </c>
+      <c r="C145" t="n">
+        <v>15</v>
+      </c>
+      <c r="D145" t="n">
+        <v>724</v>
+      </c>
+      <c r="E145" t="n">
+        <v>5</v>
+      </c>
+      <c r="F145" t="n">
+        <v>21</v>
+      </c>
+      <c r="G145" t="n">
+        <v>15</v>
+      </c>
+      <c r="H145" t="n">
+        <v>30</v>
+      </c>
+      <c r="I145" t="n">
+        <v>336</v>
+      </c>
+      <c r="J145" t="n">
+        <v>358</v>
+      </c>
+      <c r="K145" t="n">
+        <v>17</v>
+      </c>
+      <c r="L145" t="n">
+        <v>336</v>
+      </c>
+      <c r="M145" t="n">
+        <v>366</v>
+      </c>
+      <c r="N145" t="n">
+        <v>371</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajuste do horário da ultima atualização e horário de criação do gráfico
</commit_message>
<xml_diff>
--- a/Corona/uti_agregado_diario_imputada_adulto.xlsx
+++ b/Corona/uti_agregado_diario_imputada_adulto.xlsx
@@ -6744,31 +6744,31 @@
         <v>5</v>
       </c>
       <c r="F145" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G145" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H145" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I145" t="n">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="J145" t="n">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="K145" t="n">
         <v>17</v>
       </c>
       <c r="L145" t="n">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="M145" t="n">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="N145" t="n">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit após ajustes da legenda do gráfico
</commit_message>
<xml_diff>
--- a/Corona/uti_agregado_diario_imputada_adulto.xlsx
+++ b/Corona/uti_agregado_diario_imputada_adulto.xlsx
@@ -6771,6 +6771,50 @@
         <v>368</v>
       </c>
     </row>
+    <row r="146">
+      <c r="A146" s="1" t="n">
+        <v>44053</v>
+      </c>
+      <c r="B146" t="n">
+        <v>823</v>
+      </c>
+      <c r="C146" t="n">
+        <v>17</v>
+      </c>
+      <c r="D146" t="n">
+        <v>728</v>
+      </c>
+      <c r="E146" t="n">
+        <v>9</v>
+      </c>
+      <c r="F146" t="n">
+        <v>25</v>
+      </c>
+      <c r="G146" t="n">
+        <v>15</v>
+      </c>
+      <c r="H146" t="n">
+        <v>34</v>
+      </c>
+      <c r="I146" t="n">
+        <v>338</v>
+      </c>
+      <c r="J146" t="n">
+        <v>356</v>
+      </c>
+      <c r="K146" t="n">
+        <v>17</v>
+      </c>
+      <c r="L146" t="n">
+        <v>338</v>
+      </c>
+      <c r="M146" t="n">
+        <v>372</v>
+      </c>
+      <c r="N146" t="n">
+        <v>381</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>